<commit_message>
Enabled LINUX mouse support
- Fix: Mouse dragging support in DRV_TOUCH_SDL
- Fix: Config Guide spreadsheet for DRV_TOUCH_SDL cases
</commit_message>
<xml_diff>
--- a/docs/GUIslice_config_guide.xlsx
+++ b/docs/GUIslice_config_guide.xlsx
@@ -29,7 +29,31 @@
     <author>Cal</author>
   </authors>
   <commentList>
-    <comment ref="E12" authorId="0" shapeId="0">
+    <comment ref="F13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Cal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Use rpi-fbcp to mirror /dev/fb0 to /dev/fb1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +77,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="G15" authorId="0" shapeId="0">
+    <comment ref="I14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Cal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Thanks to Kevin Gordon at www.rescuerobot.org</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L23" authorId="0" shapeId="0">
+    <comment ref="N25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -101,7 +149,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G33" authorId="0" shapeId="0">
+    <comment ref="I35" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -125,7 +173,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B44" authorId="0" shapeId="0">
+    <comment ref="B46" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -149,7 +197,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B45" authorId="0" shapeId="0">
+    <comment ref="B47" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -173,7 +221,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B46" authorId="0" shapeId="0">
+    <comment ref="B48" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -202,7 +250,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="149">
   <si>
     <t>Arduino Pro Mini</t>
   </si>
@@ -325,9 +373,6 @@
   </si>
   <si>
     <t>LINUX</t>
-  </si>
-  <si>
-    <t>Prog Interface:</t>
   </si>
   <si>
     <t>GSLC_DEV_FB</t>
@@ -631,9 +676,6 @@
     <t>(mouse)</t>
   </si>
   <si>
-    <t>(RPi)</t>
-  </si>
-  <si>
     <t>Mouse</t>
   </si>
   <si>
@@ -641,6 +683,42 @@
   </si>
   <si>
     <t>DRV_SDL_MOUSE_SHOW</t>
+  </si>
+  <si>
+    <t>""</t>
+  </si>
+  <si>
+    <t>(RPi - shell)</t>
+  </si>
+  <si>
+    <t>(RPi - Xwindows)</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>"/dev/fb0" ?</t>
+  </si>
+  <si>
+    <t>SDL1.2 in shell</t>
+  </si>
+  <si>
+    <t>SDL2 in shell</t>
+  </si>
+  <si>
+    <t>SDL2 in Xwindows</t>
+  </si>
+  <si>
+    <t>Use rpi-fbcp</t>
+  </si>
+  <si>
+    <t>Programming Interface:</t>
+  </si>
+  <si>
+    <t>SDL1.2 in shell?</t>
+  </si>
+  <si>
+    <t>Special Notes</t>
   </si>
 </sst>
 </file>
@@ -763,7 +841,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -800,6 +878,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -829,7 +913,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -888,6 +972,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1205,56 +1295,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U70"/>
+  <dimension ref="A1:W72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="E37" sqref="E37"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="18.85546875" style="4" customWidth="1"/>
-    <col min="3" max="7" width="18" style="4" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" style="4" customWidth="1"/>
-    <col min="9" max="12" width="20.42578125" style="4" customWidth="1"/>
-    <col min="13" max="15" width="19.42578125" style="4" customWidth="1"/>
-    <col min="16" max="21" width="9.140625" style="4"/>
-    <col min="22" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="9" width="18" style="4" customWidth="1"/>
+    <col min="10" max="10" width="19.85546875" style="4" customWidth="1"/>
+    <col min="11" max="14" width="20.42578125" style="4" customWidth="1"/>
+    <col min="15" max="17" width="19.42578125" style="4" customWidth="1"/>
+    <col min="18" max="23" width="9.140625" style="4"/>
+    <col min="24" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="J2" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="K2" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="H2" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="I2" s="20" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
@@ -1268,31 +1358,37 @@
         <v>39</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>131</v>
+        <v>39</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="H5" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="K5" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="L5" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="M5" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="N5" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="K5" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="L5" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
       <c r="O5" s="8"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
         <v>2</v>
       </c>
@@ -1303,366 +1399,394 @@
         <v>31</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>65</v>
+        <v>131</v>
       </c>
       <c r="H6" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="J6" s="14" t="s">
         <v>31</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>70</v>
       </c>
       <c r="K6" s="14" t="s">
         <v>30</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>88</v>
+        <v>69</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>69</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B8" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D8" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="I8" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B8" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="J8" s="6" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="O8" s="6" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P8" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B9" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B10" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B11" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B12" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="J9" s="6" t="s">
+      <c r="J12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B13" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B14" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="K9" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B10" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="M10" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B11" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="L11" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B12" s="5" t="s">
+      <c r="C14" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="D14" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="H14" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="I14" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="E12" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="I12" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="J12" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="K12" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="L12" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="M12" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="N12" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="O12" s="17" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B14" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="K14" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="L14" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B15" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>63</v>
-      </c>
+      <c r="J14" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="K14" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="L14" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="M14" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="N14" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="O14" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="P14" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q14" s="23" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
@@ -1671,62 +1795,88 @@
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
       <c r="O15" s="8"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="M16" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="N16" s="8" t="s">
+        <v>61</v>
+      </c>
       <c r="O16" s="8"/>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B17" s="5" t="s">
-        <v>41</v>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>28</v>
+        <v>129</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="L17" s="8" t="s">
-        <v>32</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
       <c r="O17" s="8"/>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -1741,135 +1891,151 @@
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
+        <v>146</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L19" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="M19" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N19" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="O19" s="8"/>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B20" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
-      <c r="H20" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="J20" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="K20" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="L20" s="8" t="s">
-        <v>95</v>
-      </c>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
       <c r="M20" s="8"/>
       <c r="N20" s="8"/>
       <c r="O20" s="8"/>
-    </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B21" s="3" t="s">
-        <v>24</v>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B21" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
-      <c r="H21" s="8" t="s">
-        <v>25</v>
-      </c>
+      <c r="H21" s="8"/>
       <c r="I21" s="8"/>
-      <c r="J21" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>98</v>
-      </c>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
       <c r="N21" s="8"/>
       <c r="O21" s="8"/>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
-      <c r="H22" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I22" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="J22" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="K22" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="L22" s="11" t="s">
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L22" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
+      <c r="M22" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="N22" s="8" t="s">
+        <v>94</v>
+      </c>
       <c r="O22" s="8"/>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
-      <c r="H23" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>36</v>
-      </c>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
       <c r="J23" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="K23" s="8" t="s">
-        <v>36</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="K23" s="8"/>
       <c r="L23" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="M23" s="8"/>
+        <v>97</v>
+      </c>
+      <c r="M23" s="8" t="s">
+        <v>97</v>
+      </c>
       <c r="N23" s="8"/>
       <c r="O23" s="8"/>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B24" s="7"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8"/>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B24" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
@@ -1877,14 +2043,29 @@
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
+      <c r="J24" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K24" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L24" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="M24" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="N24" s="11" t="s">
+        <v>95</v>
+      </c>
       <c r="O24" s="8"/>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B25" s="7"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
@@ -1892,17 +2073,27 @@
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
+      <c r="J25" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K25" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L25" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="M25" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="N25" s="8" t="s">
+        <v>36</v>
+      </c>
       <c r="O25" s="8"/>
-    </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B26" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="8"/>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B26" s="7"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
@@ -1914,134 +2105,101 @@
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
       <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
       <c r="O26" s="8"/>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B27" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="H27" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="J27" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="K27" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="L27" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="M27" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="N27" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="O27" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B28" s="3" t="s">
-        <v>117</v>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B27" s="7"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="8"/>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B28" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
-      <c r="H28" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="J28" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="K28" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="L28" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M28" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="N28" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="O28" s="17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="8"/>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B29" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>137</v>
+        <v>51</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>100</v>
+        <v>46</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>100</v>
+        <v>46</v>
       </c>
       <c r="M29" s="8" t="s">
-        <v>92</v>
+        <v>46</v>
       </c>
       <c r="N29" s="8" t="s">
-        <v>100</v>
+        <v>46</v>
       </c>
       <c r="O29" s="8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="P29" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q29" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B30" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -2050,48 +2208,90 @@
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
       <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B31" s="3"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="J30" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="K30" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="L30" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="M30" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N30" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="O30" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="P30" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q30" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B31" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L31" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="M31" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="N31" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="O31" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="P31" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q31" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B32" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>55</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
@@ -2100,24 +2300,16 @@
       <c r="M32" s="8"/>
       <c r="N32" s="8"/>
       <c r="O32" s="8"/>
-    </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B33" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>51</v>
-      </c>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="8"/>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B33" s="3"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
       <c r="E33" s="8"/>
-      <c r="F33" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G33" s="12" t="s">
-        <v>64</v>
-      </c>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
@@ -2126,278 +2318,320 @@
       <c r="M33" s="8"/>
       <c r="N33" s="8"/>
       <c r="O33" s="8"/>
-    </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="P33" s="8"/>
+      <c r="Q33" s="8"/>
+    </row>
+    <row r="34" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B34" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C34" s="8">
-        <v>1</v>
-      </c>
-      <c r="D34" s="8">
-        <v>0</v>
-      </c>
-      <c r="E34" s="8">
-        <v>1</v>
-      </c>
-      <c r="F34" s="8">
-        <v>1</v>
-      </c>
-      <c r="G34" s="8">
-        <v>1</v>
-      </c>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
+        <v>41</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
       <c r="M34" s="8"/>
       <c r="N34" s="8"/>
       <c r="O34" s="8"/>
-    </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8"/>
+    </row>
+    <row r="35" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B35" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C35" s="8">
-        <v>0</v>
-      </c>
-      <c r="D35" s="8">
-        <v>0</v>
-      </c>
-      <c r="E35" s="8">
-        <v>1</v>
-      </c>
-      <c r="F35" s="8">
-        <v>0</v>
-      </c>
-      <c r="G35" s="8">
-        <v>0</v>
-      </c>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
+        <v>42</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I35" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="J35" s="8"/>
       <c r="K35" s="8"/>
       <c r="L35" s="8"/>
       <c r="M35" s="8"/>
       <c r="N35" s="8"/>
       <c r="O35" s="8"/>
-    </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="P35" s="8"/>
+      <c r="Q35" s="8"/>
+    </row>
+    <row r="36" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B36" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C36" s="8">
         <v>1</v>
       </c>
       <c r="D36" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E36" s="8">
         <v>1</v>
       </c>
       <c r="F36" s="8">
+        <v>0</v>
+      </c>
+      <c r="G36" s="8">
+        <v>0</v>
+      </c>
+      <c r="H36" s="8">
         <v>1</v>
       </c>
-      <c r="G36" s="8">
+      <c r="I36" s="8">
         <v>1</v>
       </c>
-      <c r="H36" s="8">
-        <v>0</v>
-      </c>
-      <c r="I36" s="8">
-        <v>0</v>
-      </c>
-      <c r="J36" s="8">
-        <v>0</v>
-      </c>
-      <c r="K36" s="8">
-        <v>0</v>
-      </c>
-      <c r="L36" s="8">
-        <v>0</v>
-      </c>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
       <c r="O36" s="8"/>
-    </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B37" s="3"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="8"/>
+    </row>
+    <row r="37" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B37" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C37" s="8">
+        <v>0</v>
+      </c>
+      <c r="D37" s="8">
+        <v>0</v>
+      </c>
+      <c r="E37" s="8">
+        <v>1</v>
+      </c>
+      <c r="F37" s="8">
+        <v>1</v>
+      </c>
+      <c r="G37" s="8">
+        <v>1</v>
+      </c>
+      <c r="H37" s="8">
+        <v>0</v>
+      </c>
+      <c r="I37" s="8">
+        <v>0</v>
+      </c>
       <c r="J37" s="8"/>
       <c r="K37" s="8"/>
       <c r="L37" s="8"/>
       <c r="M37" s="8"/>
       <c r="N37" s="8"/>
       <c r="O37" s="8"/>
-    </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B38" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
-      <c r="N38" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="8"/>
+    </row>
+    <row r="38" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B38" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" s="8">
+        <v>1</v>
+      </c>
+      <c r="D38" s="8">
+        <v>1</v>
+      </c>
+      <c r="E38" s="8">
+        <v>1</v>
+      </c>
+      <c r="F38" s="8">
+        <v>1</v>
+      </c>
+      <c r="G38" s="8">
+        <v>1</v>
+      </c>
+      <c r="H38" s="8">
+        <v>1</v>
+      </c>
+      <c r="I38" s="8">
+        <v>1</v>
+      </c>
+      <c r="J38" s="8">
+        <v>0</v>
+      </c>
+      <c r="K38" s="8">
+        <v>0</v>
+      </c>
+      <c r="L38" s="8">
+        <v>0</v>
+      </c>
+      <c r="M38" s="8">
+        <v>0</v>
+      </c>
+      <c r="N38" s="8">
+        <v>0</v>
+      </c>
       <c r="O38" s="8"/>
-    </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B39" s="18" t="s">
-        <v>3</v>
-      </c>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="8"/>
+    </row>
+    <row r="39" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B39" s="3"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
-      <c r="H39" s="8">
-        <v>10</v>
-      </c>
-      <c r="I39" s="8">
-        <v>10</v>
-      </c>
-      <c r="J39" s="11">
-        <v>53</v>
-      </c>
-      <c r="K39" s="8">
-        <v>10</v>
-      </c>
-      <c r="L39" s="8">
-        <v>10</v>
-      </c>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
       <c r="M39" s="8"/>
       <c r="N39" s="8"/>
       <c r="O39" s="8"/>
-    </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B40" s="18" t="s">
-        <v>4</v>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="8"/>
+    </row>
+    <row r="40" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B40" s="16" t="s">
+        <v>103</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
-      <c r="H40" s="8">
-        <v>9</v>
-      </c>
-      <c r="I40" s="8">
-        <v>9</v>
-      </c>
-      <c r="J40" s="11">
-        <v>47</v>
-      </c>
-      <c r="K40" s="8">
-        <v>9</v>
-      </c>
-      <c r="L40" s="8">
-        <v>9</v>
-      </c>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
       <c r="O40" s="8"/>
-    </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="P40" s="8"/>
+      <c r="Q40" s="8"/>
+    </row>
+    <row r="41" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B41" s="18" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
-      <c r="H41" s="8">
-        <v>0</v>
-      </c>
-      <c r="I41" s="8">
-        <v>0</v>
-      </c>
-      <c r="J41" s="11">
-        <v>49</v>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8">
+        <v>10</v>
       </c>
       <c r="K41" s="8">
-        <v>0</v>
-      </c>
-      <c r="L41" s="8">
-        <v>11</v>
-      </c>
-      <c r="M41" s="8"/>
-      <c r="N41" s="8"/>
+        <v>10</v>
+      </c>
+      <c r="L41" s="11">
+        <v>53</v>
+      </c>
+      <c r="M41" s="8">
+        <v>10</v>
+      </c>
+      <c r="N41" s="8">
+        <v>10</v>
+      </c>
       <c r="O41" s="8"/>
-    </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="P41" s="8"/>
+      <c r="Q41" s="8"/>
+    </row>
+    <row r="42" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B42" s="18" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
-      <c r="H42" s="8">
-        <v>4</v>
-      </c>
-      <c r="I42" s="8">
-        <v>4</v>
-      </c>
-      <c r="J42" s="11">
-        <v>48</v>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8">
+        <v>9</v>
       </c>
       <c r="K42" s="8">
-        <v>4</v>
-      </c>
-      <c r="L42" s="8">
-        <v>4</v>
-      </c>
-      <c r="M42" s="8"/>
-      <c r="N42" s="8"/>
+        <v>9</v>
+      </c>
+      <c r="L42" s="11">
+        <v>47</v>
+      </c>
+      <c r="M42" s="8">
+        <v>9</v>
+      </c>
+      <c r="N42" s="8">
+        <v>9</v>
+      </c>
       <c r="O42" s="8"/>
-    </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="P42" s="8"/>
+      <c r="Q42" s="8"/>
+    </row>
+    <row r="43" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B43" s="18" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
-      <c r="H43" s="8">
-        <v>1</v>
-      </c>
-      <c r="I43" s="8">
-        <v>1</v>
-      </c>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
       <c r="J43" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K43" s="8">
-        <v>1</v>
-      </c>
-      <c r="L43" s="8">
-        <v>1</v>
-      </c>
-      <c r="M43" s="8"/>
-      <c r="N43" s="8"/>
+        <v>0</v>
+      </c>
+      <c r="L43" s="11">
+        <v>49</v>
+      </c>
+      <c r="M43" s="8">
+        <v>0</v>
+      </c>
+      <c r="N43" s="8">
+        <v>11</v>
+      </c>
       <c r="O43" s="8"/>
-    </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="P43" s="8"/>
+      <c r="Q43" s="8"/>
+    </row>
+    <row r="44" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B44" s="18" t="s">
-        <v>112</v>
+        <v>6</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
@@ -2406,16 +2640,28 @@
       <c r="G44" s="8"/>
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
-      <c r="J44" s="8"/>
-      <c r="K44" s="8"/>
-      <c r="L44" s="8"/>
-      <c r="M44" s="8"/>
-      <c r="N44" s="8"/>
+      <c r="J44" s="8">
+        <v>4</v>
+      </c>
+      <c r="K44" s="8">
+        <v>4</v>
+      </c>
+      <c r="L44" s="11">
+        <v>48</v>
+      </c>
+      <c r="M44" s="8">
+        <v>4</v>
+      </c>
+      <c r="N44" s="8">
+        <v>4</v>
+      </c>
       <c r="O44" s="8"/>
-    </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="P44" s="8"/>
+      <c r="Q44" s="8"/>
+    </row>
+    <row r="45" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B45" s="18" t="s">
-        <v>113</v>
+        <v>7</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
@@ -2424,16 +2670,28 @@
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
       <c r="I45" s="8"/>
-      <c r="J45" s="8"/>
-      <c r="K45" s="8"/>
-      <c r="L45" s="8"/>
-      <c r="M45" s="8"/>
-      <c r="N45" s="8"/>
+      <c r="J45" s="8">
+        <v>1</v>
+      </c>
+      <c r="K45" s="8">
+        <v>1</v>
+      </c>
+      <c r="L45" s="8">
+        <v>1</v>
+      </c>
+      <c r="M45" s="8">
+        <v>1</v>
+      </c>
+      <c r="N45" s="8">
+        <v>1</v>
+      </c>
       <c r="O45" s="8"/>
-    </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B46" s="18" t="s">
-        <v>114</v>
+      <c r="P45" s="8"/>
+      <c r="Q45" s="8"/>
+    </row>
+    <row r="46" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B46" s="22" t="s">
+        <v>111</v>
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
@@ -2448,54 +2706,52 @@
       <c r="M46" s="8"/>
       <c r="N46" s="8"/>
       <c r="O46" s="8"/>
-    </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B47" s="18" t="s">
-        <v>8</v>
+      <c r="P46" s="8"/>
+      <c r="Q46" s="8"/>
+    </row>
+    <row r="47" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B47" s="22" t="s">
+        <v>112</v>
       </c>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
-      <c r="H47" s="8">
-        <v>0</v>
-      </c>
-      <c r="I47" s="11">
-        <v>1</v>
-      </c>
-      <c r="J47" s="8">
-        <v>0</v>
-      </c>
-      <c r="K47" s="11">
-        <v>1</v>
-      </c>
-      <c r="L47" s="8">
-        <v>0</v>
-      </c>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="8"/>
+      <c r="L47" s="8"/>
       <c r="M47" s="8"/>
       <c r="N47" s="8"/>
       <c r="O47" s="8"/>
-    </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B48" s="3"/>
+      <c r="P47" s="8"/>
+      <c r="Q47" s="8"/>
+    </row>
+    <row r="48" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B48" s="22" t="s">
+        <v>113</v>
+      </c>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
-      <c r="I48" s="17"/>
+      <c r="I48" s="8"/>
       <c r="J48" s="8"/>
-      <c r="K48" s="17"/>
+      <c r="K48" s="8"/>
       <c r="L48" s="8"/>
       <c r="M48" s="8"/>
       <c r="N48" s="8"/>
       <c r="O48" s="8"/>
-    </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B49" s="16" t="s">
-        <v>101</v>
+      <c r="P48" s="8"/>
+      <c r="Q48" s="8"/>
+    </row>
+    <row r="49" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B49" s="18" t="s">
+        <v>8</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
@@ -2504,87 +2760,93 @@
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>
       <c r="I49" s="8"/>
-      <c r="J49" s="8"/>
-      <c r="K49" s="8"/>
-      <c r="L49" s="8"/>
-      <c r="M49" s="8"/>
-      <c r="N49" s="8"/>
+      <c r="J49" s="8">
+        <v>0</v>
+      </c>
+      <c r="K49" s="11">
+        <v>1</v>
+      </c>
+      <c r="L49" s="8">
+        <v>0</v>
+      </c>
+      <c r="M49" s="11">
+        <v>1</v>
+      </c>
+      <c r="N49" s="8">
+        <v>0</v>
+      </c>
       <c r="O49" s="8"/>
-    </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B50" s="18" t="s">
-        <v>9</v>
-      </c>
+      <c r="P49" s="8"/>
+      <c r="Q49" s="8"/>
+    </row>
+    <row r="50" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B50" s="3"/>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
       <c r="G50" s="8"/>
-      <c r="H50" s="8">
-        <v>1</v>
-      </c>
-      <c r="I50" s="8">
-        <v>1</v>
-      </c>
+      <c r="H50" s="8"/>
+      <c r="I50" s="8"/>
       <c r="J50" s="8"/>
-      <c r="K50" s="8">
-        <v>1</v>
-      </c>
+      <c r="K50" s="17"/>
       <c r="L50" s="8"/>
-      <c r="M50" s="8"/>
+      <c r="M50" s="17"/>
       <c r="N50" s="8"/>
       <c r="O50" s="8"/>
-    </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B51" s="18" t="s">
-        <v>10</v>
+      <c r="P50" s="8"/>
+      <c r="Q50" s="8"/>
+    </row>
+    <row r="51" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B51" s="16" t="s">
+        <v>100</v>
       </c>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
       <c r="G51" s="8"/>
-      <c r="H51" s="8">
-        <v>1</v>
-      </c>
-      <c r="I51" s="8">
-        <v>0</v>
-      </c>
+      <c r="H51" s="8"/>
+      <c r="I51" s="8"/>
       <c r="J51" s="8"/>
-      <c r="K51" s="8">
-        <v>0</v>
-      </c>
+      <c r="K51" s="8"/>
       <c r="L51" s="8"/>
       <c r="M51" s="8"/>
       <c r="N51" s="8"/>
       <c r="O51" s="8"/>
-    </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="P51" s="8"/>
+      <c r="Q51" s="8"/>
+    </row>
+    <row r="52" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B52" s="18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
       <c r="E52" s="8"/>
       <c r="F52" s="8"/>
       <c r="G52" s="8"/>
-      <c r="H52" s="8">
-        <v>0</v>
-      </c>
-      <c r="I52" s="8">
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8">
         <v>1</v>
       </c>
-      <c r="J52" s="8"/>
       <c r="K52" s="8">
         <v>1</v>
       </c>
       <c r="L52" s="8"/>
-      <c r="M52" s="8"/>
+      <c r="M52" s="8">
+        <v>1</v>
+      </c>
       <c r="N52" s="8"/>
       <c r="O52" s="8"/>
-    </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B53" s="18"/>
+      <c r="P52" s="8"/>
+      <c r="Q52" s="8"/>
+    </row>
+    <row r="53" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B53" s="18" t="s">
+        <v>10</v>
+      </c>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
       <c r="E53" s="8"/>
@@ -2592,16 +2854,24 @@
       <c r="G53" s="8"/>
       <c r="H53" s="8"/>
       <c r="I53" s="8"/>
-      <c r="J53" s="8"/>
-      <c r="K53" s="8"/>
+      <c r="J53" s="8">
+        <v>1</v>
+      </c>
+      <c r="K53" s="8">
+        <v>0</v>
+      </c>
       <c r="L53" s="8"/>
-      <c r="M53" s="8"/>
+      <c r="M53" s="8">
+        <v>0</v>
+      </c>
       <c r="N53" s="8"/>
       <c r="O53" s="8"/>
-    </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B54" s="16" t="s">
-        <v>103</v>
+      <c r="P53" s="8"/>
+      <c r="Q53" s="8"/>
+    </row>
+    <row r="54" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B54" s="18" t="s">
+        <v>11</v>
       </c>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
@@ -2610,38 +2880,42 @@
       <c r="G54" s="8"/>
       <c r="H54" s="8"/>
       <c r="I54" s="8"/>
-      <c r="J54" s="8"/>
-      <c r="K54" s="8"/>
+      <c r="J54" s="8">
+        <v>0</v>
+      </c>
+      <c r="K54" s="8">
+        <v>1</v>
+      </c>
       <c r="L54" s="8"/>
-      <c r="M54" s="8"/>
+      <c r="M54" s="8">
+        <v>1</v>
+      </c>
       <c r="N54" s="8"/>
       <c r="O54" s="8"/>
-    </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B55" s="18" t="s">
-        <v>115</v>
-      </c>
+      <c r="P54" s="8"/>
+      <c r="Q54" s="8"/>
+    </row>
+    <row r="55" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B55" s="18"/>
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
       <c r="E55" s="8"/>
       <c r="F55" s="8"/>
       <c r="G55" s="8"/>
       <c r="H55" s="8"/>
-      <c r="I55" s="10">
-        <v>0</v>
-      </c>
-      <c r="J55" s="10"/>
-      <c r="K55" s="10">
-        <v>0</v>
-      </c>
-      <c r="L55" s="10"/>
+      <c r="I55" s="8"/>
+      <c r="J55" s="8"/>
+      <c r="K55" s="8"/>
+      <c r="L55" s="8"/>
       <c r="M55" s="8"/>
       <c r="N55" s="8"/>
       <c r="O55" s="8"/>
-    </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B56" s="18" t="s">
-        <v>12</v>
+      <c r="P55" s="8"/>
+      <c r="Q55" s="8"/>
+    </row>
+    <row r="56" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B56" s="16" t="s">
+        <v>102</v>
       </c>
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
@@ -2649,21 +2923,19 @@
       <c r="F56" s="8"/>
       <c r="G56" s="8"/>
       <c r="H56" s="8"/>
-      <c r="I56" s="10">
-        <v>1</v>
-      </c>
-      <c r="J56" s="10"/>
-      <c r="K56" s="10">
-        <v>1</v>
-      </c>
-      <c r="L56" s="10"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="8"/>
+      <c r="K56" s="8"/>
+      <c r="L56" s="8"/>
       <c r="M56" s="8"/>
       <c r="N56" s="8"/>
       <c r="O56" s="8"/>
-    </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="P56" s="8"/>
+      <c r="Q56" s="8"/>
+    </row>
+    <row r="57" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B57" s="18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
@@ -2671,21 +2943,23 @@
       <c r="F57" s="8"/>
       <c r="G57" s="8"/>
       <c r="H57" s="8"/>
-      <c r="I57" s="10">
-        <v>0</v>
-      </c>
-      <c r="J57" s="10"/>
+      <c r="I57" s="8"/>
+      <c r="J57" s="8"/>
       <c r="K57" s="10">
         <v>0</v>
       </c>
       <c r="L57" s="10"/>
-      <c r="M57" s="8"/>
-      <c r="N57" s="8"/>
+      <c r="M57" s="10">
+        <v>0</v>
+      </c>
+      <c r="N57" s="10"/>
       <c r="O57" s="8"/>
-    </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="P57" s="8"/>
+      <c r="Q57" s="8"/>
+    </row>
+    <row r="58" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B58" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
@@ -2693,21 +2967,23 @@
       <c r="F58" s="8"/>
       <c r="G58" s="8"/>
       <c r="H58" s="8"/>
-      <c r="I58" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J58" s="10"/>
-      <c r="K58" s="10" t="s">
-        <v>19</v>
+      <c r="I58" s="8"/>
+      <c r="J58" s="8"/>
+      <c r="K58" s="10">
+        <v>1</v>
       </c>
       <c r="L58" s="10"/>
-      <c r="M58" s="8"/>
-      <c r="N58" s="8"/>
+      <c r="M58" s="10">
+        <v>1</v>
+      </c>
+      <c r="N58" s="10"/>
       <c r="O58" s="8"/>
-    </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="P58" s="8"/>
+      <c r="Q58" s="8"/>
+    </row>
+    <row r="59" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B59" s="18" t="s">
-        <v>14</v>
+        <v>115</v>
       </c>
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
@@ -2715,21 +2991,23 @@
       <c r="F59" s="8"/>
       <c r="G59" s="8"/>
       <c r="H59" s="8"/>
-      <c r="I59" s="10">
-        <v>8</v>
-      </c>
-      <c r="J59" s="10"/>
+      <c r="I59" s="8"/>
+      <c r="J59" s="8"/>
       <c r="K59" s="10">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="L59" s="10"/>
-      <c r="M59" s="8"/>
-      <c r="N59" s="8"/>
+      <c r="M59" s="10">
+        <v>0</v>
+      </c>
+      <c r="N59" s="10"/>
       <c r="O59" s="8"/>
-    </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="P59" s="8"/>
+      <c r="Q59" s="8"/>
+    </row>
+    <row r="60" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B60" s="18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
@@ -2737,21 +3015,23 @@
       <c r="F60" s="8"/>
       <c r="G60" s="8"/>
       <c r="H60" s="8"/>
-      <c r="I60" s="11">
-        <v>230</v>
-      </c>
-      <c r="J60" s="10"/>
-      <c r="K60" s="11">
-        <v>230</v>
+      <c r="I60" s="8"/>
+      <c r="J60" s="8"/>
+      <c r="K60" s="10" t="s">
+        <v>19</v>
       </c>
       <c r="L60" s="10"/>
-      <c r="M60" s="8"/>
-      <c r="N60" s="8"/>
+      <c r="M60" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N60" s="10"/>
       <c r="O60" s="8"/>
-    </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="P60" s="8"/>
+      <c r="Q60" s="8"/>
+    </row>
+    <row r="61" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B61" s="18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
@@ -2759,21 +3039,23 @@
       <c r="F61" s="8"/>
       <c r="G61" s="8"/>
       <c r="H61" s="8"/>
-      <c r="I61" s="11">
-        <v>260</v>
-      </c>
-      <c r="J61" s="10"/>
-      <c r="K61" s="11">
-        <v>260</v>
+      <c r="I61" s="8"/>
+      <c r="J61" s="8"/>
+      <c r="K61" s="10">
+        <v>8</v>
       </c>
       <c r="L61" s="10"/>
-      <c r="M61" s="8"/>
-      <c r="N61" s="8"/>
+      <c r="M61" s="10">
+        <v>8</v>
+      </c>
+      <c r="N61" s="10"/>
       <c r="O61" s="8"/>
-    </row>
-    <row r="62" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="P61" s="8"/>
+      <c r="Q61" s="8"/>
+    </row>
+    <row r="62" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B62" s="18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C62" s="8"/>
       <c r="D62" s="8"/>
@@ -2781,21 +3063,23 @@
       <c r="F62" s="8"/>
       <c r="G62" s="8"/>
       <c r="H62" s="8"/>
-      <c r="I62" s="11">
-        <v>3800</v>
-      </c>
-      <c r="J62" s="10"/>
+      <c r="I62" s="8"/>
+      <c r="J62" s="8"/>
       <c r="K62" s="11">
-        <v>3800</v>
+        <v>230</v>
       </c>
       <c r="L62" s="10"/>
-      <c r="M62" s="8"/>
-      <c r="N62" s="8"/>
+      <c r="M62" s="11">
+        <v>230</v>
+      </c>
+      <c r="N62" s="10"/>
       <c r="O62" s="8"/>
-    </row>
-    <row r="63" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="P62" s="8"/>
+      <c r="Q62" s="8"/>
+    </row>
+    <row r="63" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B63" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
@@ -2803,100 +3087,158 @@
       <c r="F63" s="8"/>
       <c r="G63" s="8"/>
       <c r="H63" s="8"/>
-      <c r="I63" s="11">
+      <c r="I63" s="8"/>
+      <c r="J63" s="8"/>
+      <c r="K63" s="11">
+        <v>260</v>
+      </c>
+      <c r="L63" s="10"/>
+      <c r="M63" s="11">
+        <v>260</v>
+      </c>
+      <c r="N63" s="10"/>
+      <c r="O63" s="8"/>
+      <c r="P63" s="8"/>
+      <c r="Q63" s="8"/>
+    </row>
+    <row r="64" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B64" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="8"/>
+      <c r="G64" s="8"/>
+      <c r="H64" s="8"/>
+      <c r="I64" s="8"/>
+      <c r="J64" s="8"/>
+      <c r="K64" s="11">
+        <v>3800</v>
+      </c>
+      <c r="L64" s="10"/>
+      <c r="M64" s="11">
+        <v>3800</v>
+      </c>
+      <c r="N64" s="10"/>
+      <c r="O64" s="8"/>
+      <c r="P64" s="8"/>
+      <c r="Q64" s="8"/>
+    </row>
+    <row r="65" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B65" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C65" s="8"/>
+      <c r="D65" s="8"/>
+      <c r="E65" s="8"/>
+      <c r="F65" s="8"/>
+      <c r="G65" s="8"/>
+      <c r="H65" s="8"/>
+      <c r="I65" s="8"/>
+      <c r="J65" s="8"/>
+      <c r="K65" s="11">
         <v>3700</v>
       </c>
-      <c r="J63" s="10"/>
-      <c r="K63" s="11">
+      <c r="L65" s="10"/>
+      <c r="M65" s="11">
         <v>3700</v>
       </c>
-      <c r="L63" s="10"/>
-      <c r="M63" s="8"/>
-      <c r="N63" s="8"/>
-      <c r="O63" s="8"/>
-    </row>
-    <row r="64" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B64" s="18"/>
-      <c r="C64" s="9"/>
-      <c r="D64" s="9"/>
-      <c r="E64" s="9"/>
-      <c r="F64" s="9"/>
-      <c r="G64" s="9"/>
-      <c r="H64" s="9"/>
-      <c r="I64" s="9"/>
-      <c r="J64" s="9"/>
-      <c r="K64" s="9"/>
-      <c r="L64" s="9"/>
-      <c r="M64" s="8"/>
-      <c r="N64" s="8"/>
-      <c r="O64" s="8"/>
-    </row>
-    <row r="65" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B65" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="C65" s="9"/>
-      <c r="D65" s="9"/>
-      <c r="E65" s="9"/>
-      <c r="F65" s="9"/>
-      <c r="G65" s="9"/>
-      <c r="H65" s="9"/>
-      <c r="I65" s="9"/>
-      <c r="J65" s="9"/>
-      <c r="K65" s="9"/>
-      <c r="L65" s="9"/>
-      <c r="M65" s="8"/>
-      <c r="N65" s="8"/>
+      <c r="N65" s="10"/>
       <c r="O65" s="8"/>
-    </row>
-    <row r="66" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B66" s="18" t="s">
+      <c r="P65" s="8"/>
+      <c r="Q65" s="8"/>
+    </row>
+    <row r="66" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B66" s="18"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="9"/>
+      <c r="H66" s="9"/>
+      <c r="I66" s="9"/>
+      <c r="J66" s="9"/>
+      <c r="K66" s="9"/>
+      <c r="L66" s="9"/>
+      <c r="M66" s="9"/>
+      <c r="N66" s="9"/>
+      <c r="O66" s="8"/>
+      <c r="P66" s="8"/>
+      <c r="Q66" s="8"/>
+    </row>
+    <row r="67" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B67" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
+      <c r="G67" s="9"/>
+      <c r="H67" s="9"/>
+      <c r="I67" s="9"/>
+      <c r="J67" s="9"/>
+      <c r="K67" s="9"/>
+      <c r="L67" s="9"/>
+      <c r="M67" s="9"/>
+      <c r="N67" s="9"/>
+      <c r="O67" s="8"/>
+      <c r="P67" s="8"/>
+      <c r="Q67" s="8"/>
+    </row>
+    <row r="68" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B68" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C66" s="8"/>
-      <c r="D66" s="8"/>
-      <c r="E66" s="8"/>
-      <c r="F66" s="8"/>
-      <c r="G66" s="8"/>
-      <c r="H66" s="11">
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8"/>
+      <c r="H68" s="8"/>
+      <c r="I68" s="8"/>
+      <c r="J68" s="11">
         <v>40</v>
       </c>
-      <c r="I66" s="8"/>
-      <c r="J66" s="8"/>
-      <c r="K66" s="8"/>
-      <c r="L66" s="8"/>
-      <c r="M66" s="8"/>
-      <c r="N66" s="8"/>
-      <c r="O66" s="8"/>
-    </row>
-    <row r="67" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B67" s="3"/>
-      <c r="C67" s="8"/>
-      <c r="D67" s="8"/>
-      <c r="E67" s="8"/>
-      <c r="F67" s="8"/>
-      <c r="G67" s="8"/>
-      <c r="H67" s="8"/>
-      <c r="I67" s="8"/>
-      <c r="J67" s="8"/>
-      <c r="K67" s="8"/>
-      <c r="L67" s="8"/>
-      <c r="M67" s="8"/>
-      <c r="N67" s="8"/>
-      <c r="O67" s="8"/>
-    </row>
-    <row r="70" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B70" s="4" t="s">
+      <c r="K68" s="8"/>
+      <c r="L68" s="8"/>
+      <c r="M68" s="8"/>
+      <c r="N68" s="8"/>
+      <c r="O68" s="8"/>
+      <c r="P68" s="8"/>
+      <c r="Q68" s="8"/>
+    </row>
+    <row r="69" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B69" s="3"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+      <c r="E69" s="8"/>
+      <c r="F69" s="8"/>
+      <c r="G69" s="8"/>
+      <c r="H69" s="8"/>
+      <c r="I69" s="8"/>
+      <c r="J69" s="8"/>
+      <c r="K69" s="8"/>
+      <c r="L69" s="8"/>
+      <c r="M69" s="8"/>
+      <c r="N69" s="8"/>
+      <c r="O69" s="8"/>
+      <c r="P69" s="8"/>
+      <c r="Q69" s="8"/>
+    </row>
+    <row r="72" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B72" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C72" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="I2" r:id="rId2"/>
+    <hyperlink ref="K2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId3"/>

</xml_diff>